<commit_message>
added cross category relationship comparasion
</commit_message>
<xml_diff>
--- a/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
+++ b/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3018</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2893</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2147</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1301</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>704</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>581</v>
+        <v>599</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +578,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kitchen &amp; Dining</t>
+          <t>Seasonal &amp; Holidays</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +593,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Seasonal &amp; Holidays</t>
+          <t>Kitchen &amp; Dining</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing the model worked
</commit_message>
<xml_diff>
--- a/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
+++ b/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3022</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2145</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1301</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1175</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>692</v>
+        <v>701</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10">
@@ -582,22 +582,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>423</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Home Decor</t>
+          <t>Textiles &amp; Cozy Items</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Seasonal &amp; Holidays</t>
+          <t>Textiles &amp; Cozy Items</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last run of model and deleted negative sampling
</commit_message>
<xml_diff>
--- a/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
+++ b/Results/first_third/first_third_word2vec_top_category_combinations.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2039</v>
+        <v>8264</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1829</v>
+        <v>8252</v>
       </c>
     </row>
     <row r="4">
@@ -492,67 +492,67 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>998</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Seasonal &amp; Holidays</t>
+          <t>Home Decor</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Seasonal &amp; Holidays</t>
+          <t>Kitchen &amp; Dining</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>661</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kids &amp; Toys</t>
+          <t>Kitchen &amp; Dining</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kids &amp; Toys</t>
+          <t>Home Decor</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>561</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Party Supplies</t>
+          <t>Seasonal &amp; Holidays</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Party Supplies</t>
+          <t>Seasonal &amp; Holidays</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>380</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Garden &amp; Outdoor</t>
+          <t>Kids &amp; Toys</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Garden &amp; Outdoor</t>
+          <t>Kids &amp; Toys</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>313</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="9">
@@ -563,41 +563,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Kitchen &amp; Dining</t>
+          <t>Seasonal &amp; Holidays</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>310</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fashion &amp; Accessories</t>
+          <t>Seasonal &amp; Holidays</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fashion &amp; Accessories</t>
+          <t>Home Decor</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>293</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kitchen &amp; Dining</t>
+          <t>Home Decor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Home Decor</t>
+          <t>Stationery &amp; Office</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>293</v>
+        <v>1843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>